<commit_message>
You can now update the quantity of a book! yay!!!!
</commit_message>
<xml_diff>
--- a/Team7_SPSUBookstore/Team7_SPSUBookstore/Resources/books.xlsx
+++ b/Team7_SPSUBookstore/Team7_SPSUBookstore/Resources/books.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24526"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Y:\Code\IntroSWE\Team7_SPSUBookstore\Team7_SPSUBookstore\Resources\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2500" yWindow="1620" windowWidth="22320" windowHeight="12480" tabRatio="123"/>
+    <workbookView xWindow="2505" yWindow="1620" windowWidth="22320" windowHeight="12480" tabRatio="123"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -975,6 +980,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1308,24 +1316,24 @@
       <selection activeCell="J45" sqref="J45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.33203125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="13.375" style="1" customWidth="1"/>
     <col min="2" max="2" width="15" customWidth="1"/>
     <col min="3" max="3" width="23" customWidth="1"/>
-    <col min="4" max="4" width="12.6640625" customWidth="1"/>
+    <col min="4" max="4" width="12.625" customWidth="1"/>
     <col min="6" max="6" width="11" style="1"/>
     <col min="8" max="8" width="11" style="1"/>
-    <col min="9" max="9" width="13.1640625" customWidth="1"/>
-    <col min="10" max="10" width="13.6640625" customWidth="1"/>
-    <col min="11" max="11" width="12.33203125" customWidth="1"/>
+    <col min="9" max="9" width="13.125" customWidth="1"/>
+    <col min="10" max="10" width="13.625" customWidth="1"/>
+    <col min="11" max="11" width="12.375" customWidth="1"/>
     <col min="12" max="12" width="14.5" customWidth="1"/>
-    <col min="13" max="13" width="14.33203125" customWidth="1"/>
+    <col min="13" max="13" width="14.375" customWidth="1"/>
     <col min="14" max="14" width="11" customWidth="1"/>
-    <col min="18" max="18" width="70.83203125" customWidth="1"/>
+    <col min="18" max="18" width="70.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" s="4" customFormat="1" ht="16.5" thickBot="1">
+    <row r="1" spans="1:18" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
@@ -1381,7 +1389,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:18" s="6" customFormat="1" ht="51.75">
+    <row r="2" spans="1:18" s="6" customFormat="1" ht="51.75" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>44</v>
       </c>
@@ -1410,7 +1418,7 @@
         <v>57</v>
       </c>
       <c r="J2" s="8">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="K2" s="8">
         <v>35</v>
@@ -1419,7 +1427,7 @@
         <v>58</v>
       </c>
       <c r="M2" s="8">
-        <v>999999</v>
+        <v>54</v>
       </c>
       <c r="N2" s="13">
         <v>160</v>
@@ -1437,7 +1445,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="3" spans="1:18" s="6" customFormat="1" ht="39">
+    <row r="3" spans="1:18" s="6" customFormat="1" ht="39" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>45</v>
       </c>
@@ -1493,7 +1501,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="4" spans="1:18" s="6" customFormat="1" ht="39">
+    <row r="4" spans="1:18" s="6" customFormat="1" ht="39" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>97</v>
       </c>
@@ -1549,7 +1557,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="5" spans="1:18" s="6" customFormat="1" ht="77.25">
+    <row r="5" spans="1:18" s="6" customFormat="1" ht="77.25" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>46</v>
       </c>
@@ -1605,7 +1613,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="6" spans="1:18" s="6" customFormat="1" ht="26.25">
+    <row r="6" spans="1:18" s="6" customFormat="1" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>136</v>
       </c>
@@ -1661,7 +1669,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="7" spans="1:18" s="6" customFormat="1" ht="26.25">
+    <row r="7" spans="1:18" s="6" customFormat="1" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>71</v>
       </c>
@@ -1717,7 +1725,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="8" spans="1:18" s="6" customFormat="1" ht="26.25">
+    <row r="8" spans="1:18" s="6" customFormat="1" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>76</v>
       </c>
@@ -1773,7 +1781,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="9" spans="1:18" s="6" customFormat="1" ht="39">
+    <row r="9" spans="1:18" s="6" customFormat="1" ht="39" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>137</v>
       </c>
@@ -1829,7 +1837,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="10" spans="1:18" s="6" customFormat="1" ht="102.75">
+    <row r="10" spans="1:18" s="6" customFormat="1" ht="102.75" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>200</v>
       </c>
@@ -1885,7 +1893,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="11" spans="1:18" ht="26.25">
+    <row r="11" spans="1:18" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>94</v>
       </c>
@@ -1941,7 +1949,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="12" spans="1:18" ht="39">
+    <row r="12" spans="1:18" ht="39" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>95</v>
       </c>
@@ -1997,7 +2005,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="13" spans="1:18" ht="64.5">
+    <row r="13" spans="1:18" ht="64.5" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>199</v>
       </c>
@@ -2053,7 +2061,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="14" spans="1:18" ht="77.25">
+    <row r="14" spans="1:18" ht="77.25" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>138</v>
       </c>
@@ -2109,7 +2117,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="15" spans="1:18" ht="26.25">
+    <row r="15" spans="1:18" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>73</v>
       </c>
@@ -2165,7 +2173,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="16" spans="1:18" ht="26.25">
+    <row r="16" spans="1:18" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>48</v>
       </c>
@@ -2221,7 +2229,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="17" spans="1:18" ht="39">
+    <row r="17" spans="1:18" ht="39" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>41</v>
       </c>
@@ -2277,7 +2285,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="18" spans="1:18" ht="51.75">
+    <row r="18" spans="1:18" ht="51.75" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>96</v>
       </c>
@@ -2333,7 +2341,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="19" spans="1:18" ht="39">
+    <row r="19" spans="1:18" ht="39" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>201</v>
       </c>
@@ -2389,7 +2397,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="20" spans="1:18" ht="12">
+    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>70</v>
       </c>
@@ -2445,7 +2453,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="21" spans="1:18" ht="39">
+    <row r="21" spans="1:18" ht="39" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>42</v>
       </c>
@@ -2501,7 +2509,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="22" spans="1:18" ht="26.25">
+    <row r="22" spans="1:18" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>139</v>
       </c>
@@ -2557,7 +2565,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="23" spans="1:18" ht="39">
+    <row r="23" spans="1:18" ht="39" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>198</v>
       </c>
@@ -2613,7 +2621,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="24" spans="1:18" ht="26.25">
+    <row r="24" spans="1:18" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>98</v>
       </c>
@@ -2669,7 +2677,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="25" spans="1:18" ht="39">
+    <row r="25" spans="1:18" ht="39" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>43</v>
       </c>
@@ -2725,7 +2733,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="26" spans="1:18" ht="26.25">
+    <row r="26" spans="1:18" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>140</v>
       </c>
@@ -2781,7 +2789,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="27" spans="1:18" ht="26.25">
+    <row r="27" spans="1:18" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
         <v>206</v>
       </c>
@@ -2837,7 +2845,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="28" spans="1:18" ht="51.75">
+    <row r="28" spans="1:18" ht="51.75" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
         <v>205</v>
       </c>
@@ -2893,7 +2901,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="29" spans="1:18" ht="26.25">
+    <row r="29" spans="1:18" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
         <v>99</v>
       </c>
@@ -2949,7 +2957,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="30" spans="1:18" ht="77.25">
+    <row r="30" spans="1:18" ht="77.25" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
         <v>141</v>
       </c>
@@ -3005,7 +3013,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="31" spans="1:18" ht="12">
+    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
         <v>142</v>
       </c>
@@ -3061,7 +3069,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="32" spans="1:18" ht="39">
+    <row r="32" spans="1:18" ht="39" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
         <v>74</v>
       </c>
@@ -3117,7 +3125,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="33" spans="1:18" ht="51.75">
+    <row r="33" spans="1:18" ht="51.75" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
         <v>75</v>
       </c>
@@ -3173,7 +3181,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="34" spans="1:18" ht="39">
+    <row r="34" spans="1:18" ht="39" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
         <v>72</v>
       </c>
@@ -3229,7 +3237,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="35" spans="1:18" ht="39">
+    <row r="35" spans="1:18" ht="39" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
         <v>77</v>
       </c>
@@ -3285,7 +3293,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="36" spans="1:18" ht="51.75">
+    <row r="36" spans="1:18" ht="51.75" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
         <v>143</v>
       </c>
@@ -3341,7 +3349,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="37" spans="1:18" ht="26.25">
+    <row r="37" spans="1:18" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
         <v>203</v>
       </c>
@@ -3397,7 +3405,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="38" spans="1:18" ht="26.25">
+    <row r="38" spans="1:18" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
         <v>49</v>
       </c>
@@ -3453,7 +3461,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="39" spans="1:18" ht="12">
+    <row r="39" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
         <v>204</v>
       </c>
@@ -3509,7 +3517,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="40" spans="1:18" ht="26.25">
+    <row r="40" spans="1:18" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
         <v>207</v>
       </c>
@@ -3565,7 +3573,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="41" spans="1:18" ht="51.75">
+    <row r="41" spans="1:18" ht="51.75" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
         <v>40</v>
       </c>
@@ -3621,7 +3629,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="42" spans="1:18" ht="26.25">
+    <row r="42" spans="1:18" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
         <v>202</v>
       </c>
@@ -3677,7 +3685,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="43" spans="1:18" ht="64.5">
+    <row r="43" spans="1:18" ht="64.5" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
         <v>100</v>
       </c>
@@ -3733,7 +3741,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="44" spans="1:18" ht="26.25">
+    <row r="44" spans="1:18" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
         <v>144</v>
       </c>
@@ -3789,7 +3797,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="45" spans="1:18" ht="49">
+    <row r="45" spans="1:18" ht="51.75" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
         <v>47</v>
       </c>

</xml_diff>

<commit_message>
Fixes some of the excel process issues.
</commit_message>
<xml_diff>
--- a/Team7_SPSUBookstore/Team7_SPSUBookstore/Resources/books.xlsx
+++ b/Team7_SPSUBookstore/Team7_SPSUBookstore/Resources/books.xlsx
@@ -1418,7 +1418,7 @@
         <v>57</v>
       </c>
       <c r="J2" s="8">
-        <v>57</v>
+        <v>0</v>
       </c>
       <c r="K2" s="8">
         <v>35</v>
@@ -1645,7 +1645,7 @@
         <v>50</v>
       </c>
       <c r="K6" s="8">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="L6" s="8">
         <v>50</v>

</xml_diff>